<commit_message>
implement roles for all views
</commit_message>
<xml_diff>
--- a/database/LookUps/Roles.xlsx
+++ b/database/LookUps/Roles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\personal\private-work\El-Mostakbal-Technology\MoH-web-portal\database\LookUps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2C3BA3-E0D8-4912-ADD3-5B3037BA3076}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C55E93B-1ACA-4970-8CCD-680135412D1A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7E175BF0-DE7F-4DAC-A67D-85CBE1B1A992}"/>
   </bookViews>
@@ -594,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7E8E3BB-9F18-420F-9474-AFB94FFD6224}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>